<commit_message>
update perubahan struktur upload template excel
</commit_message>
<xml_diff>
--- a/public/referensi/template upload data.xlsx
+++ b/public/referensi/template upload data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\application_letters\public\referensi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1817522D-7769-4F20-9731-2A8B163E8DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8A6451-0AC6-46D4-89C5-0299E3F3616B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{6CA4C54B-CC02-43B2-9E43-2B376088AE04}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
   <si>
     <t>Pilih Narasumber dan Moderator</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Pilih Peserta</t>
-  </si>
-  <si>
-    <t>Jabatan - Lembaga</t>
   </si>
   <si>
     <t>Dosen Uin Sunan Kalijaga Yogyakarta</t>
@@ -192,9 +189,6 @@
     </r>
   </si>
   <si>
-    <t>NOTE :</t>
-  </si>
-  <si>
     <r>
       <t>Nama</t>
     </r>
@@ -224,6 +218,30 @@
   <si>
     <t>Dosen MIT</t>
   </si>
+  <si>
+    <t>NIP</t>
+  </si>
+  <si>
+    <t>Jabatan Fungsional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Pangkat (Golongan)</t>
+  </si>
+  <si>
+    <t>Peran Kepanitiaan</t>
+  </si>
+  <si>
+    <t>19787xxxxxx</t>
+  </si>
+  <si>
+    <t>Pembina (IV/A)</t>
+  </si>
+  <si>
+    <t>Lektor Kepala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Pangkat (Golongan) </t>
+  </si>
 </sst>
 </file>
 
@@ -235,7 +253,7 @@
     <numFmt numFmtId="166" formatCode="[$Rp-421]#,##0"/>
     <numFmt numFmtId="167" formatCode="_-[$Rp-421]* #,##0_-;\-[$Rp-421]* #,##0_-;_-[$Rp-421]* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,6 +278,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -296,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -307,13 +333,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="167" formatCode="_-[$Rp-421]* #,##0_-;\-[$Rp-421]* #,##0_-;_-[$Rp-421]* &quot;-&quot;_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="[$Rp-421]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="hh:mm:ss;@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="166" formatCode="[$Rp-421]#,##0"/>
@@ -334,54 +369,63 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1AD992B8-EE0D-4B3F-97A5-0828F24BF435}" name="Table1" displayName="Table1" ref="A2:D6" totalsRowShown="0">
-  <autoFilter ref="A2:D6" xr:uid="{1AD992B8-EE0D-4B3F-97A5-0828F24BF435}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1AD992B8-EE0D-4B3F-97A5-0828F24BF435}" name="Table1" displayName="Table1" ref="A2:G6" totalsRowShown="0">
+  <autoFilter ref="A2:G6" xr:uid="{1AD992B8-EE0D-4B3F-97A5-0828F24BF435}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{6C044829-B420-4801-8CA4-DA5709091451}" name="No"/>
     <tableColumn id="2" xr3:uid="{DC6A4271-0F86-45C4-BA1E-6651B0ABBBB9}" name="Nama*"/>
-    <tableColumn id="3" xr3:uid="{B0829CC5-ADCE-4FA7-A381-782E894794E6}" name="Jabatan-Lembaga"/>
-    <tableColumn id="4" xr3:uid="{D5EF2A06-6525-469E-A4A1-39337A158571}" name="Peran"/>
+    <tableColumn id="3" xr3:uid="{B0829CC5-ADCE-4FA7-A381-782E894794E6}" name="NIP"/>
+    <tableColumn id="4" xr3:uid="{D5EF2A06-6525-469E-A4A1-39337A158571}" name="  Pangkat (Golongan) "/>
+    <tableColumn id="5" xr3:uid="{F876FCF8-A9E9-4189-A9E3-47AC0B780C9A}" name="Jabatan Fungsional"/>
+    <tableColumn id="6" xr3:uid="{2CBFE367-0EAB-4012-9233-14CF5EDFEBFC}" name="Jabatan-Lembaga"/>
+    <tableColumn id="7" xr3:uid="{8E7EE526-D1C8-41D2-BF64-05E9CABD263C}" name="Peran"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9115CEC8-3514-4270-A722-F14CCB56E7F7}" name="Table2" displayName="Table2" ref="G2:I9" totalsRowShown="0">
-  <autoFilter ref="G2:I9" xr:uid="{9115CEC8-3514-4270-A722-F14CCB56E7F7}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{20436BCA-F8B7-4BCC-9160-D730129AABC5}" name="No"/>
-    <tableColumn id="2" xr3:uid="{6D4A7AFD-0427-42D8-B298-7575E1EC7008}" name="Peran"/>
-    <tableColumn id="3" xr3:uid="{01A3CC04-DD46-4A6E-A43E-11825F8ED104}" name="Nama"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B144F879-42A2-46D1-9A61-02C16C7DD87C}" name="Table2" displayName="Table2" ref="J2:O9" totalsRowShown="0">
+  <autoFilter ref="J2:O9" xr:uid="{B144F879-42A2-46D1-9A61-02C16C7DD87C}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{6AC94064-DE95-42D9-BD4F-9079B5928DC6}" name="No"/>
+    <tableColumn id="2" xr3:uid="{178A532B-EA58-43AB-8906-757F962C8811}" name="Peran Kepanitiaan"/>
+    <tableColumn id="3" xr3:uid="{7D43EB72-5F4B-4E46-ACAD-FF1D280D660D}" name="Nama"/>
+    <tableColumn id="4" xr3:uid="{F08EC938-7A88-4EC9-90DB-5DD84D79C3A5}" name="NIP"/>
+    <tableColumn id="5" xr3:uid="{509EF18A-5C0E-495A-BA27-6FDBECCC85DC}" name="  Pangkat (Golongan)"/>
+    <tableColumn id="6" xr3:uid="{4AD892A8-A699-46DF-98FF-902B51F91094}" name="Jabatan Fungsional"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6E4FC7FF-D11D-4BEF-A01C-79B87D1BF661}" name="Table25" displayName="Table25" ref="L2:N9" totalsRowShown="0">
-  <autoFilter ref="L2:N9" xr:uid="{6E4FC7FF-D11D-4BEF-A01C-79B87D1BF661}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{BBF37881-D4D5-4C67-A570-AE740C8B0A0D}" name="No"/>
-    <tableColumn id="2" xr3:uid="{820EA3D9-5F45-4698-B7D4-FC09D7909142}" name="Nama*"/>
-    <tableColumn id="3" xr3:uid="{9764B332-1AD2-4719-AE69-A3C579B1507F}" name="Jabatan - Lembaga"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{040DD02B-896D-406F-A320-A8CDE7768D73}" name="Table25" displayName="Table25" ref="R2:W9" totalsRowShown="0">
+  <autoFilter ref="R2:W9" xr:uid="{040DD02B-896D-406F-A320-A8CDE7768D73}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{7087207C-84C7-4F49-9EE7-DC30A2152048}" name="No"/>
+    <tableColumn id="2" xr3:uid="{32C25856-EC7C-4422-8FF8-B772B08DF8BC}" name="Nama*"/>
+    <tableColumn id="3" xr3:uid="{168160FE-E0AE-4E84-9755-5F7336A2E76F}" name="NIP" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{AAE5EBAE-DED0-4228-B8F0-33A13664E24E}" name="  Pangkat (Golongan)"/>
+    <tableColumn id="5" xr3:uid="{83D83657-DB50-42DF-972F-3D20C2E1B987}" name="Jabatan Fungsional"/>
+    <tableColumn id="6" xr3:uid="{BC4121DE-97AE-4115-928A-4A13C854C6FA}" name="Jabatan-Lembaga" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{765E37C4-EC21-4A19-9B60-D6A75C01F7A7}" name="Table3" displayName="Table3" ref="Q2:X10" totalsRowShown="0">
-  <autoFilter ref="Q2:X10" xr:uid="{765E37C4-EC21-4A19-9B60-D6A75C01F7A7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{161F963C-5713-460C-B4D6-4D22E81BC56A}" name="Table3" displayName="Table3" ref="Z2:AG10" totalsRowShown="0">
+  <autoFilter ref="Z2:AG10" xr:uid="{161F963C-5713-460C-B4D6-4D22E81BC56A}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D12B7DD3-4D10-4D3F-AFA0-02D845B1CA50}" name="No"/>
-    <tableColumn id="2" xr3:uid="{02B0E304-7B47-4C74-88AA-FEFC1C4F7903}" name="Kode*"/>
-    <tableColumn id="3" xr3:uid="{82850E34-84FA-42DD-AE52-DE82CA9F79AC}" name="Uraian*"/>
-    <tableColumn id="4" xr3:uid="{F6D2FB4C-C845-452F-865A-28271B5D961B}" name="Sub Uraian"/>
-    <tableColumn id="5" xr3:uid="{FE731B4F-DB28-490C-B2F9-4F0967AAA8F0}" name="Volume"/>
-    <tableColumn id="6" xr3:uid="{B35ED2FB-5420-4812-A0DD-9EE29C9E88B9}" name="Satuan"/>
-    <tableColumn id="7" xr3:uid="{088546B4-3035-4609-AD28-5713FDFD053A}" name="Harga Satuan" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{562310F5-FC31-4E95-BBE6-F3200F59D8B4}" name="Jumlah" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E3B0A244-F9CC-4F68-9C46-57C9313895D9}" name="No"/>
+    <tableColumn id="2" xr3:uid="{4001FABE-36D5-4D8A-82BA-48A20952C67B}" name="Kode*"/>
+    <tableColumn id="3" xr3:uid="{56AFCB5A-50D2-45F7-BF86-F0BE7E98F379}" name="Uraian*"/>
+    <tableColumn id="4" xr3:uid="{ACD97E41-FACD-4DAA-A998-67BC7AF17B01}" name="Sub Uraian"/>
+    <tableColumn id="5" xr3:uid="{89D970A1-991B-46FE-B519-7A86371E0305}" name="Volume"/>
+    <tableColumn id="6" xr3:uid="{459E3245-8AE0-461B-98EA-B693D23910AF}" name="Satuan"/>
+    <tableColumn id="7" xr3:uid="{9AB1A501-5EC8-4501-9C93-8E2BD76257E0}" name="Harga Satuan" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{DC732125-F649-44BC-8EA2-F0C4AB3C34AF}" name="Jumlah" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -704,134 +748,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B59B9331-4B57-4138-BDB9-703DEB8172AA}">
-  <dimension ref="A1:AG10"/>
+  <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.21875" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.5546875" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" customWidth="1"/>
-    <col min="7" max="7" width="7.77734375" customWidth="1"/>
-    <col min="8" max="8" width="23.88671875" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" customWidth="1"/>
-    <col min="11" max="11" width="13.109375" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" customWidth="1"/>
-    <col min="13" max="13" width="17.44140625" customWidth="1"/>
-    <col min="14" max="14" width="23.44140625" customWidth="1"/>
-    <col min="15" max="15" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" customWidth="1"/>
+    <col min="3" max="3" width="37.21875" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.77734375" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.21875" customWidth="1"/>
+    <col min="13" max="13" width="26.5546875" customWidth="1"/>
+    <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.88671875" customWidth="1"/>
     <col min="17" max="17" width="9.5546875" customWidth="1"/>
-    <col min="18" max="18" width="16.21875" style="3" customWidth="1"/>
-    <col min="19" max="19" width="13" style="4" customWidth="1"/>
-    <col min="20" max="20" width="13.33203125" style="4" customWidth="1"/>
-    <col min="21" max="21" width="17.21875" customWidth="1"/>
-    <col min="22" max="22" width="44.33203125" customWidth="1"/>
-    <col min="23" max="23" width="13.6640625" customWidth="1"/>
+    <col min="18" max="18" width="5.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.6640625" style="4" customWidth="1"/>
+    <col min="21" max="21" width="19" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="34" customWidth="1"/>
     <col min="24" max="24" width="23" customWidth="1"/>
-    <col min="26" max="26" width="7" customWidth="1"/>
-    <col min="27" max="27" width="17.88671875" customWidth="1"/>
-    <col min="28" max="28" width="28.6640625" customWidth="1"/>
-    <col min="29" max="29" width="37.109375" customWidth="1"/>
-    <col min="30" max="31" width="10.21875" customWidth="1"/>
-    <col min="32" max="32" width="10.21875" style="5" customWidth="1"/>
-    <col min="33" max="33" width="14.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="37.6640625" customWidth="1"/>
+    <col min="30" max="30" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="21.88671875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:33" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
-      <c r="G1" s="7" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
-      <c r="O1" s="2"/>
+      <c r="O1" s="7"/>
       <c r="P1" s="2"/>
-      <c r="Q1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="R1" s="7"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="S1" s="7"/>
       <c r="T1" s="7"/>
       <c r="U1" s="7"/>
       <c r="V1" s="7"/>
       <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
+      <c r="X1" s="8"/>
+      <c r="Z1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="7"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" t="s">
         <v>2</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" t="s">
+        <v>50</v>
+      </c>
+      <c r="R2" t="s">
         <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" t="s">
-        <v>42</v>
       </c>
       <c r="S2" t="s">
         <v>43</v>
       </c>
       <c r="T2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U2" t="s">
+        <v>51</v>
+      </c>
+      <c r="V2" t="s">
+        <v>50</v>
+      </c>
+      <c r="W2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD2" t="s">
         <v>28</v>
       </c>
-      <c r="U2" t="s">
+      <c r="AE2" t="s">
         <v>29</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AF2" t="s">
         <v>30</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AG2" t="s">
         <v>31</v>
       </c>
-      <c r="X2" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -839,303 +923,329 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="G3">
+      <c r="J3">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" t="s">
+      <c r="L3" t="s">
         <v>5</v>
       </c>
-      <c r="L3">
+      <c r="M3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O3" t="s">
+        <v>53</v>
+      </c>
+      <c r="R3">
         <v>1</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="S3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O3" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q3">
+      <c r="W3" t="s">
+        <v>20</v>
+      </c>
+      <c r="X3" s="6"/>
+      <c r="Z3">
         <v>1</v>
       </c>
-      <c r="R3" t="s">
+      <c r="AA3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB3" t="s">
         <v>33</v>
       </c>
-      <c r="S3" t="s">
-        <v>34</v>
-      </c>
-      <c r="T3"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="6"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
         <v>10</v>
       </c>
-      <c r="G4">
+      <c r="J4">
         <v>2</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
         <v>13</v>
       </c>
-      <c r="I4" t="s">
+      <c r="L4" t="s">
         <v>8</v>
       </c>
-      <c r="L4">
+      <c r="M4" s="10"/>
+      <c r="R4">
         <v>2</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q4">
+      <c r="S4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W4" t="s">
+        <v>20</v>
+      </c>
+      <c r="X4" s="6"/>
+      <c r="Z4">
         <v>2</v>
       </c>
-      <c r="R4">
+      <c r="AA4">
         <v>525112</v>
       </c>
-      <c r="S4" t="s">
+      <c r="AB4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC4" t="s">
         <v>35</v>
       </c>
-      <c r="T4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U4">
+      <c r="AD4">
         <v>170</v>
       </c>
-      <c r="V4" t="s">
-        <v>41</v>
-      </c>
-      <c r="W4" s="5">
+      <c r="AE4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF4" s="5">
         <v>30000</v>
       </c>
-      <c r="X4" s="6">
-        <f>U4*W4</f>
+      <c r="AG4" s="6">
+        <f>AD4*AF4</f>
         <v>5100000</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>7</v>
       </c>
-      <c r="G5">
+      <c r="J5">
         <v>3</v>
       </c>
-      <c r="H5" t="s">
+      <c r="K5" t="s">
         <v>17</v>
       </c>
-      <c r="I5" t="s">
+      <c r="L5" t="s">
         <v>14</v>
       </c>
-      <c r="L5">
+      <c r="M5" s="10"/>
+      <c r="R5">
         <v>3</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="S5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W5" t="s">
+        <v>20</v>
+      </c>
+      <c r="X5" s="6"/>
+      <c r="Z5">
+        <v>3</v>
+      </c>
+      <c r="AA5">
+        <v>525112</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD5">
+        <v>170</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF5" s="5">
+        <v>15000</v>
+      </c>
+      <c r="AG5" s="6">
+        <f>AD5*AF5</f>
+        <v>2550000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="10"/>
+      <c r="R6">
+        <v>4</v>
+      </c>
+      <c r="S6" s="1"/>
+      <c r="W6" t="s">
+        <v>20</v>
+      </c>
+      <c r="X6" s="6"/>
+      <c r="Z6">
+        <v>4</v>
+      </c>
+      <c r="AA6">
+        <v>525113</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD6">
+        <v>3</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF6" s="5">
+        <v>900000</v>
+      </c>
+      <c r="AG6" s="6">
+        <f>AD6*AF6</f>
+        <v>2700000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="10"/>
+      <c r="R7">
+        <v>5</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W7" t="s">
+        <v>20</v>
+      </c>
+      <c r="X7" s="6"/>
+      <c r="Z7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="10"/>
+      <c r="R8">
+        <v>6</v>
+      </c>
+      <c r="S8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N5" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q5">
-        <v>3</v>
-      </c>
-      <c r="R5">
-        <v>525112</v>
-      </c>
-      <c r="S5" t="s">
-        <v>35</v>
-      </c>
-      <c r="T5" t="s">
-        <v>37</v>
-      </c>
-      <c r="U5">
-        <v>170</v>
-      </c>
-      <c r="V5" t="s">
-        <v>41</v>
-      </c>
-      <c r="W5" s="5">
-        <v>15000</v>
-      </c>
-      <c r="X5" s="6">
-        <f>U5*W5</f>
-        <v>2550000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6">
-        <v>4</v>
-      </c>
-      <c r="M6" s="1"/>
-      <c r="N6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q6">
-        <v>4</v>
-      </c>
-      <c r="R6">
-        <v>525113</v>
-      </c>
-      <c r="S6" t="s">
-        <v>38</v>
-      </c>
-      <c r="T6" t="s">
-        <v>39</v>
-      </c>
-      <c r="U6">
-        <v>3</v>
-      </c>
-      <c r="V6" t="s">
-        <v>40</v>
-      </c>
-      <c r="W6" s="5">
-        <v>900000</v>
-      </c>
-      <c r="X6" s="6">
-        <f>U6*W6</f>
-        <v>2700000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7">
-        <v>5</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q7">
-        <v>5</v>
-      </c>
-      <c r="R7"/>
-      <c r="S7"/>
-      <c r="T7"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="6"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="G8">
-        <v>6</v>
-      </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8">
-        <v>6</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N8" t="s">
-        <v>21</v>
-      </c>
-      <c r="R8"/>
-      <c r="S8"/>
-      <c r="T8"/>
-      <c r="W8" s="5"/>
+      <c r="W8" t="s">
+        <v>20</v>
+      </c>
       <c r="X8" s="6"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="H9" t="s">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="K9" t="s">
         <v>17</v>
       </c>
-      <c r="I9" t="s">
+      <c r="L9" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" s="10"/>
+      <c r="R9">
+        <v>7</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W9" t="s">
         <v>48</v>
       </c>
-      <c r="L9">
-        <v>7</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N9" t="s">
-        <v>50</v>
-      </c>
-      <c r="R9"/>
-      <c r="S9"/>
-      <c r="T9"/>
-      <c r="W9" s="5"/>
       <c r="X9" s="6"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="R10"/>
       <c r="S10"/>
       <c r="T10"/>
       <c r="W10" s="5"/>
       <c r="X10" s="6"/>
     </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="AF15"/>
+      <c r="AG15"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="Q1:X1"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="Z1:AG1"/>
+    <mergeCell ref="R1:W1"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="J1:O1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation operator="notBetween" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R1:R1048576" xr:uid="{0AFB3C9C-5ED2-477C-BB53-2FA3CC1D7BBE}"/>
+    <dataValidation operator="notBetween" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R1 AA1:AA10 R10:R14 R16:R1048576" xr:uid="{0AFB3C9C-5ED2-477C-BB53-2FA3CC1D7BBE}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>